<commit_message>
added data in excel
</commit_message>
<xml_diff>
--- a/src/Data/Business.xlsx
+++ b/src/Data/Business.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samik\OneDrive\Documents\NetBeansProjects\assignment-4-xeroxstrategists\src\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A68B320-8A68-433E-899D-AB3610E2046D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3403A788-3370-426E-920E-AE5BBDC3937A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{7299C4BE-89C8-E240-A97E-9F08726DA00B}"/>
   </bookViews>
@@ -441,13 +441,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -765,7 +763,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -775,10 +773,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" t="s">
         <v>73</v>
       </c>
     </row>

</xml_diff>